<commit_message>
debuging code de thomas pour Q2
</commit_message>
<xml_diff>
--- a/data/datasetFinal.xlsx
+++ b/data/datasetFinal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/floriandubois/Documents/GitHub/TFE_horaires_FPMS/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/floriandubois/Documents/GitHub/Horraire-Polytech/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69E3F69-26A4-0F44-8BA3-ECD31EDFB978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872A3FD7-AA7C-114B-B4E3-0597D00F7C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27700" windowHeight="15960" tabRatio="589" xr2:uid="{CFDF16B8-0417-47BD-9E0F-F29B352C84DD}"/>
   </bookViews>
@@ -2962,10 +2962,10 @@
   <dimension ref="A1:AI125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C110" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="S23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C111" sqref="C111"/>
+      <selection pane="bottomRight" activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2975,14 +2975,15 @@
     <col min="3" max="3" width="26.5" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="28.1640625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" style="11" customWidth="1"/>
-    <col min="8" max="9" width="13.1640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="1.83203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="11" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="11" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="0.1640625" style="11" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0.1640625" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" customWidth="1"/>
-    <col min="12" max="12" width="47.6640625" customWidth="1"/>
-    <col min="13" max="13" width="34.6640625" customWidth="1"/>
-    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.1640625" customWidth="1"/>
+    <col min="13" max="13" width="2.83203125" customWidth="1"/>
+    <col min="14" max="14" width="21.5" customWidth="1"/>
     <col min="15" max="16" width="12.1640625" customWidth="1"/>
     <col min="17" max="17" width="6.83203125" customWidth="1"/>
     <col min="18" max="18" width="14.1640625" customWidth="1"/>

</xml_diff>

<commit_message>
CPplacer fini MES COUILLES ! (oui j'en avais marre)
</commit_message>
<xml_diff>
--- a/data/datasetFinal.xlsx
+++ b/data/datasetFinal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/floriandubois/Documents/GitHub/Horraire-Polytech/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FE8CC8-66C5-A347-B29D-A32AC732F291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F764A5F0-AD9B-0B42-9BF2-C8C101FF2AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27700" windowHeight="15960" tabRatio="589" activeTab="2" xr2:uid="{CFDF16B8-0417-47BD-9E0F-F29B352C84DD}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27700" windowHeight="15960" tabRatio="589" activeTab="1" xr2:uid="{CFDF16B8-0417-47BD-9E0F-F29B352C84DD}"/>
   </bookViews>
   <sheets>
     <sheet name="TFE" sheetId="11" r:id="rId1"/>
@@ -2247,157 +2247,157 @@
     <t>totalStudents</t>
   </si>
   <si>
-    <t>MA1-CHSDM.PEE</t>
-  </si>
-  <si>
-    <t>MA1-CHSDM.GM</t>
-  </si>
-  <si>
-    <t>MA1-ELEC-FS AI &amp; SC</t>
-  </si>
-  <si>
-    <t>MA1-ELEC-FS EE &amp; SG</t>
-  </si>
-  <si>
-    <t>MA1-ELEC-FS SigSys</t>
-  </si>
-  <si>
-    <t>MA1-MECA-FS CP</t>
-  </si>
-  <si>
-    <t>MA1-MECA-FS GE</t>
-  </si>
-  <si>
-    <t>MA1-MECA- FS Mécatro</t>
-  </si>
-  <si>
-    <t>MA1 - MECA - SMACCS</t>
+    <t>weekStart</t>
+  </si>
+  <si>
+    <t>dayStart</t>
+  </si>
+  <si>
+    <t>slotStart</t>
+  </si>
+  <si>
+    <t>weekEnd</t>
+  </si>
+  <si>
+    <t>dayEnd</t>
+  </si>
+  <si>
+    <t>slotEnd</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>teacher</t>
+  </si>
+  <si>
+    <t>Zangara G</t>
+  </si>
+  <si>
+    <t>Dumont E</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>room</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>slot</t>
+  </si>
+  <si>
+    <t>I-MARO-121</t>
+  </si>
+  <si>
+    <t>Ch.1</t>
+  </si>
+  <si>
+    <t>I-ILIA-100</t>
+  </si>
+  <si>
+    <t>I-MRDV-120</t>
+  </si>
+  <si>
+    <t>I-MARO-120</t>
+  </si>
+  <si>
+    <t>I-POLY-012</t>
+  </si>
+  <si>
+    <t>V-LANG-161</t>
+  </si>
+  <si>
+    <t>I-SDMA-120</t>
+  </si>
+  <si>
+    <t>Ch.2</t>
+  </si>
+  <si>
+    <t>I-SDMA-121</t>
+  </si>
+  <si>
+    <t>I-MANA-102</t>
+  </si>
+  <si>
+    <t>V-LANG-162</t>
+  </si>
+  <si>
+    <t>I-TRMO-120</t>
+  </si>
+  <si>
+    <t>Com Fr</t>
+  </si>
+  <si>
+    <t>1er mai</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>MA1_CHSDM.PEE</t>
+  </si>
+  <si>
+    <t>MA1_CHSDM.GM</t>
+  </si>
+  <si>
+    <t>MA1_ELEC-FS AI &amp; SC</t>
+  </si>
+  <si>
+    <t>MA1_ELEC-FS EE &amp; SG</t>
+  </si>
+  <si>
+    <t>MA1_ELEC-FS SigSys</t>
+  </si>
+  <si>
+    <t>MA1_MECA-FS CP</t>
+  </si>
+  <si>
+    <t>MA1_MECA-FS GE</t>
+  </si>
+  <si>
+    <t>MA1_MECA- FS Mécatro</t>
+  </si>
+  <si>
+    <t>MA1_MECA - SMACCS</t>
   </si>
   <si>
     <t>MA1_MIN</t>
   </si>
   <si>
-    <t>MA2-CHSDM.PEE</t>
-  </si>
-  <si>
-    <t>MA2-CHSDM.GM</t>
-  </si>
-  <si>
-    <t>MA2-ELEC-FS AI &amp; SC</t>
-  </si>
-  <si>
-    <t>MA2-ELEC-FS EE &amp; SG</t>
-  </si>
-  <si>
-    <t>MA2-ELEC-FS SigSys</t>
+    <t>MA2_CHSDM.PEE</t>
+  </si>
+  <si>
+    <t>MA2_CHSDM.GM</t>
+  </si>
+  <si>
+    <t>MA2_ELEC-FS AI &amp; SC</t>
+  </si>
+  <si>
+    <t>MA2_ELEC-FS EE &amp; SG</t>
+  </si>
+  <si>
+    <t>MA2_ELEC-FS SigSys</t>
   </si>
   <si>
     <t>MA2_IG</t>
   </si>
   <si>
-    <t>MA2-MECA-FS CP</t>
-  </si>
-  <si>
-    <t>MA2-MECA-FS GE</t>
-  </si>
-  <si>
-    <t>MA2-MECA- FS Mécatro</t>
+    <t>MA2_MECA-FS CP</t>
+  </si>
+  <si>
+    <t>MA2_MECA-FS GE</t>
+  </si>
+  <si>
+    <t>MA2_MECA- FS Mécatro</t>
   </si>
   <si>
     <t>MA2_MIN</t>
-  </si>
-  <si>
-    <t>weekStart</t>
-  </si>
-  <si>
-    <t>dayStart</t>
-  </si>
-  <si>
-    <t>slotStart</t>
-  </si>
-  <si>
-    <t>weekEnd</t>
-  </si>
-  <si>
-    <t>dayEnd</t>
-  </si>
-  <si>
-    <t>slotEnd</t>
-  </si>
-  <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
-    <t>teacher</t>
-  </si>
-  <si>
-    <t>Zangara G</t>
-  </si>
-  <si>
-    <t>Dumont E</t>
-  </si>
-  <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>room</t>
-  </si>
-  <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>slot</t>
-  </si>
-  <si>
-    <t>I-MARO-121</t>
-  </si>
-  <si>
-    <t>Ch.1</t>
-  </si>
-  <si>
-    <t>I-ILIA-100</t>
-  </si>
-  <si>
-    <t>I-MRDV-120</t>
-  </si>
-  <si>
-    <t>I-MARO-120</t>
-  </si>
-  <si>
-    <t>I-POLY-012</t>
-  </si>
-  <si>
-    <t>V-LANG-161</t>
-  </si>
-  <si>
-    <t>I-SDMA-120</t>
-  </si>
-  <si>
-    <t>Ch.2</t>
-  </si>
-  <si>
-    <t>I-SDMA-121</t>
-  </si>
-  <si>
-    <t>I-MANA-102</t>
-  </si>
-  <si>
-    <t>V-LANG-162</t>
-  </si>
-  <si>
-    <t>I-TRMO-120</t>
-  </si>
-  <si>
-    <t>Com Fr</t>
-  </si>
-  <si>
-    <t>1er mai</t>
-  </si>
-  <si>
-    <t>Q3</t>
   </si>
 </sst>
 </file>
@@ -3034,7 +3034,7 @@
   <dimension ref="A1:AI134"/>
   <sheetViews>
     <sheetView zoomScale="117" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="R57" sqref="R57"/>
@@ -11887,8 +11887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3B9CBA-18FB-49B9-8E60-DFBF3B5515D4}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11987,7 +11987,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>584</v>
+        <v>615</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -11998,7 +11998,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>585</v>
+        <v>616</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -12009,7 +12009,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>586</v>
+        <v>617</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -12020,7 +12020,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>587</v>
+        <v>618</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -12031,7 +12031,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>588</v>
+        <v>619</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -12053,7 +12053,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>589</v>
+        <v>620</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -12064,7 +12064,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>590</v>
+        <v>621</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -12075,7 +12075,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>591</v>
+        <v>622</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -12086,7 +12086,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>592</v>
+        <v>623</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -12097,7 +12097,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>593</v>
+        <v>624</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -12108,7 +12108,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>594</v>
+        <v>625</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -12119,7 +12119,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>595</v>
+        <v>626</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -12130,7 +12130,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>596</v>
+        <v>627</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -12141,7 +12141,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>597</v>
+        <v>628</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -12152,7 +12152,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>598</v>
+        <v>629</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -12163,7 +12163,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>599</v>
+        <v>630</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -12174,7 +12174,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>600</v>
+        <v>631</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -12185,7 +12185,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>601</v>
+        <v>632</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -12196,7 +12196,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>602</v>
+        <v>633</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -12207,7 +12207,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>603</v>
+        <v>634</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -12225,7 +12225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71A1E3E-FD3C-499D-AB50-9AA283081EC1}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -12239,28 +12239,28 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>604</v>
+        <v>584</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>605</v>
+        <v>585</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>606</v>
+        <v>586</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>607</v>
+        <v>587</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>608</v>
+        <v>588</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>609</v>
+        <v>589</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>610</v>
+        <v>590</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>611</v>
+        <v>591</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -12744,7 +12744,7 @@
         <v>255</v>
       </c>
       <c r="B16" t="s">
-        <v>634</v>
+        <v>614</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -12791,34 +12791,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>604</v>
+        <v>584</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>605</v>
+        <v>585</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>606</v>
+        <v>586</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>607</v>
+        <v>587</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>608</v>
+        <v>588</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>609</v>
+        <v>589</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>610</v>
+        <v>590</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>611</v>
+        <v>591</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -14863,7 +14863,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B62" t="s">
         <v>38</v>
@@ -14897,7 +14897,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B63" t="s">
         <v>38</v>
@@ -14931,7 +14931,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B64" t="s">
         <v>38</v>
@@ -14965,7 +14965,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B65" t="s">
         <v>38</v>
@@ -14999,7 +14999,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B66" t="s">
         <v>38</v>
@@ -15033,7 +15033,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B67" t="s">
         <v>38</v>
@@ -15067,7 +15067,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B68" t="s">
         <v>38</v>
@@ -15101,7 +15101,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B69" t="s">
         <v>38</v>
@@ -15135,7 +15135,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B70" t="s">
         <v>38</v>
@@ -15169,7 +15169,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B71" t="s">
         <v>38</v>
@@ -15203,7 +15203,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B72" t="s">
         <v>38</v>
@@ -15237,7 +15237,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B73" t="s">
         <v>38</v>
@@ -16903,7 +16903,7 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B122" t="s">
         <v>38</v>
@@ -16937,7 +16937,7 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B123" t="s">
         <v>38</v>
@@ -16971,7 +16971,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B124" t="s">
         <v>38</v>
@@ -17005,7 +17005,7 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B125" t="s">
         <v>38</v>
@@ -17039,7 +17039,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B126" t="s">
         <v>38</v>
@@ -17073,7 +17073,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B127" t="s">
         <v>38</v>
@@ -17107,7 +17107,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B128" t="s">
         <v>38</v>
@@ -17141,7 +17141,7 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B129" t="s">
         <v>38</v>
@@ -17175,7 +17175,7 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B130" t="s">
         <v>38</v>
@@ -17209,7 +17209,7 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B131" t="s">
         <v>38</v>
@@ -17243,7 +17243,7 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B132" t="s">
         <v>38</v>
@@ -17277,7 +17277,7 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B133" t="s">
         <v>38</v>
@@ -17331,28 +17331,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>615</v>
+        <v>595</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>616</v>
+        <v>596</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>604</v>
+        <v>584</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>607</v>
+        <v>587</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>617</v>
+        <v>597</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>618</v>
+        <v>598</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -17363,10 +17363,10 @@
         <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
       <c r="D2" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -17389,10 +17389,10 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>621</v>
+        <v>601</v>
       </c>
       <c r="D3" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -17415,10 +17415,10 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="D4" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -17441,10 +17441,10 @@
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
       <c r="D5" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -17467,10 +17467,10 @@
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>624</v>
+        <v>604</v>
       </c>
       <c r="D6" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -17487,16 +17487,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>625</v>
+        <v>605</v>
       </c>
       <c r="D7" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -17519,10 +17519,10 @@
         <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>626</v>
+        <v>606</v>
       </c>
       <c r="D8" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -17545,10 +17545,10 @@
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>628</v>
+        <v>608</v>
       </c>
       <c r="D9" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -17571,10 +17571,10 @@
         <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>629</v>
+        <v>609</v>
       </c>
       <c r="D10" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -17597,10 +17597,10 @@
         <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>630</v>
+        <v>610</v>
       </c>
       <c r="D11" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -17617,16 +17617,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>631</v>
+        <v>611</v>
       </c>
       <c r="D12" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -17662,22 +17662,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>615</v>
+        <v>595</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>616</v>
+        <v>596</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>604</v>
+        <v>584</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>607</v>
+        <v>587</v>
       </c>
       <c r="G1" s="18"/>
     </row>
@@ -17689,10 +17689,10 @@
         <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
       <c r="D2" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -17709,10 +17709,10 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>621</v>
+        <v>601</v>
       </c>
       <c r="D3" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -17729,10 +17729,10 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="D4" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -17749,10 +17749,10 @@
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
       <c r="D5" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -17769,10 +17769,10 @@
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>624</v>
+        <v>604</v>
       </c>
       <c r="D6" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -17783,16 +17783,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>625</v>
+        <v>605</v>
       </c>
       <c r="D7" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -17809,10 +17809,10 @@
         <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>626</v>
+        <v>606</v>
       </c>
       <c r="D8" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -17829,10 +17829,10 @@
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>628</v>
+        <v>608</v>
       </c>
       <c r="D9" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -17849,10 +17849,10 @@
         <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>629</v>
+        <v>609</v>
       </c>
       <c r="D10" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -17869,10 +17869,10 @@
         <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>630</v>
+        <v>610</v>
       </c>
       <c r="D11" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -17883,16 +17883,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>631</v>
+        <v>611</v>
       </c>
       <c r="D12" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -17924,33 +17924,33 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>604</v>
+        <v>584</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>605</v>
+        <v>585</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>606</v>
+        <v>586</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>607</v>
+        <v>587</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>608</v>
+        <v>588</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>609</v>
+        <v>589</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>610</v>
+        <v>590</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>611</v>
+        <v>591</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>632</v>
+        <v>612</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -17984,7 +17984,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>633</v>
+        <v>613</v>
       </c>
       <c r="B3" t="s">
         <v>350</v>

</xml_diff>

<commit_message>
modif input 60% (optimiste)
</commit_message>
<xml_diff>
--- a/data/datasetFinal.xlsx
+++ b/data/datasetFinal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/floriandubois/Documents/GitHub/Horraire-Polytech/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F764A5F0-AD9B-0B42-9BF2-C8C101FF2AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E238D4CC-B27E-DE45-9B87-2455D22A8E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27700" windowHeight="15960" tabRatio="589" activeTab="1" xr2:uid="{CFDF16B8-0417-47BD-9E0F-F29B352C84DD}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27780" windowHeight="16920" tabRatio="589" xr2:uid="{CFDF16B8-0417-47BD-9E0F-F29B352C84DD}"/>
   </bookViews>
   <sheets>
     <sheet name="TFE" sheetId="11" r:id="rId1"/>
@@ -493,7 +493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1577" uniqueCount="636">
   <si>
     <t>cursus</t>
   </si>
@@ -2398,6 +2398,9 @@
   </si>
   <si>
     <t>MA2_MIN</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -3033,11 +3036,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436D5779-576B-4D03-A998-370CA8906C1C}">
   <dimension ref="A1:AI134"/>
   <sheetViews>
-    <sheetView zoomScale="117" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AF10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R57" sqref="R57"/>
+      <selection pane="bottomRight" activeCell="AJ16" sqref="AJ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7154,7 +7157,9 @@
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
+      <c r="R57" s="1" t="s">
+        <v>635</v>
+      </c>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
@@ -11887,9 +11892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3B9CBA-18FB-49B9-8E60-DFBF3B5515D4}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12226,7 +12229,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17320,7 +17323,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17643,6 +17646,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -17911,7 +17915,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>